<commit_message>
API to bulkinsertdeeplinks , refreshDeeplinks
</commit_message>
<xml_diff>
--- a/packages/api/src/assets/deeplink.xlsx
+++ b/packages/api/src/assets/deeplink.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\apollo-hospitals\packages\api\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80468D2F-7CFE-4CF4-9BD9-3D28611C9E11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031B2968-6A6D-454A-894C-F889C82F61F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Doctor ID</t>
   </si>
@@ -49,68 +49,59 @@
     <t>Doctor patient Download</t>
   </si>
   <si>
-    <t>Apollo Doctors</t>
-  </si>
-  <si>
-    <t>A-Anandi-49212</t>
-  </si>
-  <si>
-    <t>A-1172756553</t>
-  </si>
-  <si>
-    <t>https://apl247.onelink.me/AEkA/d79452e2</t>
-  </si>
-  <si>
-    <t>d79452e2</t>
-  </si>
-  <si>
     <t>AEkA</t>
   </si>
   <si>
-    <t>c9e86fe2-2e5e-4f4d-a31c-3d486cc438d5</t>
-  </si>
-  <si>
-    <t>A-Anitha-37240</t>
-  </si>
-  <si>
     <t>A-755525673</t>
   </si>
   <si>
-    <t>https://apl247.onelink.me/AEkA/624b9ce</t>
-  </si>
-  <si>
-    <t>624b9ce</t>
-  </si>
-  <si>
-    <t>1778e721-96c8-4a6a-876a-c1df60f11be9</t>
-  </si>
-  <si>
-    <t>A-G-K-Gokhale-15381</t>
-  </si>
-  <si>
-    <t>A-4827767632</t>
-  </si>
-  <si>
-    <t>https://apl247.onelink.me/AEkA/dbbbdcd2</t>
-  </si>
-  <si>
-    <t>dbbbdcd2</t>
-  </si>
-  <si>
     <t>3d4a107b-bc5f-4dc7-b7f1-08c0897fcafc</t>
   </si>
   <si>
     <t>linkRefreshDate</t>
   </si>
   <si>
-    <t>2020-06-01T11:09:07.318Z</t>
+    <t>test1-49212</t>
+  </si>
+  <si>
+    <t>Test2-37240</t>
+  </si>
+  <si>
+    <t>d99b07e3-587b-4eaa-b188-8e7c505a492b</t>
+  </si>
+  <si>
+    <t>https://apollo247.onelink.me/MGY5/fded5b5f</t>
+  </si>
+  <si>
+    <t>C-1009839359</t>
+  </si>
+  <si>
+    <t>fded5b5f</t>
+  </si>
+  <si>
+    <t>MGY5</t>
+  </si>
+  <si>
+    <t>https://apl247.onelink.me/AEkA/1ddf36d4</t>
+  </si>
+  <si>
+    <t>1ddf36d4</t>
+  </si>
+  <si>
+    <t>Doctor Connect</t>
+  </si>
+  <si>
+    <t>DOCTOR CONNECT</t>
+  </si>
+  <si>
+    <t>2020-04-30T14:25:35.089Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +232,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,7 +542,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -586,12 +585,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -625,6 +626,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -945,18 +947,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" customWidth="1"/>
+    <col min="2" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="41.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -985,36 +989,36 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1025,57 +1029,33 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
       <c r="I3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
         <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{6CEE94A3-64D1-4DD4-B956-EC434D0C5679}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{4342F8F1-6AC1-4BA0-AA0D-E2A95DC5BB5A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>